<commit_message>
Update reader and test data due to the change of schema.
</commit_message>
<xml_diff>
--- a/test/helper/farrowing_data/farrowing_data.xlsx
+++ b/test/helper/farrowing_data/farrowing_data.xlsx
@@ -1,11 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="27904"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10509"/>
   <workbookPr/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{6466BA74-2B02-4F72-A138-6E7FF644BF2C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/huangzhangyu/Documents/大學/實驗室/種豬資料庫/breeding_DB/test/helper/farrowing_data/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F9B38B21-D494-464E-AED2-9F1AB197EB26}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="15460" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="分娩資料" sheetId="3" r:id="rId1"/>
@@ -17,23 +22,12 @@
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="762" uniqueCount="222">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="763" uniqueCount="223">
   <si>
     <t>生日年品種耳號</t>
   </si>
@@ -699,6 +693,10 @@
   </si>
   <si>
     <t>1017-3</t>
+  </si>
+  <si>
+    <t>胎號</t>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
 </file>
@@ -706,14 +704,21 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="[$-F400]h:mm:ss\ AM/PM"/>
+    <numFmt numFmtId="176" formatCode="[$-F400]h:mm:ss\ AM/PM"/>
   </numFmts>
-  <fonts count="1">
+  <fonts count="2">
     <font>
       <sz val="12"/>
       <color theme="1"/>
       <name val="新細明體"/>
       <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <name val="新細明體"/>
+      <family val="3"/>
+      <charset val="136"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -740,7 +745,7 @@
   <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="一般" xfId="0" builtinId="0"/>
@@ -1075,22 +1080,23 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4C6E5BEE-6ACF-40EF-BC29-1914A85A0815}">
-  <dimension ref="A1:L63"/>
+  <dimension ref="A1:M63"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A42" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="L64" sqref="L64"/>
+      <pane ySplit="1" topLeftCell="A34" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="M2" sqref="M2:M63"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="16.5"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="15.125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="15.1640625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="9.5" bestFit="1" customWidth="1"/>
     <col min="5" max="9" width="3" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="17.25" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="17.1640625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="9.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12">
+    <row r="1" spans="1:13">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1127,8 +1133,11 @@
       <c r="L1" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="2" spans="1:12">
+      <c r="M1" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13">
       <c r="A2" t="s">
         <v>12</v>
       </c>
@@ -1162,8 +1171,12 @@
       <c r="K2" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="3" spans="1:12">
+      <c r="M2">
+        <f ca="1">RANDBETWEEN(1000, 2000)</f>
+        <v>1950</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13">
       <c r="A3" t="s">
         <v>12</v>
       </c>
@@ -1197,8 +1210,12 @@
       <c r="K3" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="4" spans="1:12">
+      <c r="M3">
+        <f t="shared" ref="M3:M63" ca="1" si="0">RANDBETWEEN(1000, 2000)</f>
+        <v>1241</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13">
       <c r="A4" t="s">
         <v>15</v>
       </c>
@@ -1232,8 +1249,12 @@
       <c r="K4" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="5" spans="1:12">
+      <c r="M4">
+        <f t="shared" ca="1" si="0"/>
+        <v>1833</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13">
       <c r="A5" t="s">
         <v>16</v>
       </c>
@@ -1267,8 +1288,12 @@
       <c r="K5" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="6" spans="1:12">
+      <c r="M5">
+        <f t="shared" ca="1" si="0"/>
+        <v>1078</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13">
       <c r="A6" t="s">
         <v>16</v>
       </c>
@@ -1302,8 +1327,12 @@
       <c r="K6" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="7" spans="1:12">
+      <c r="M6">
+        <f t="shared" ca="1" si="0"/>
+        <v>1769</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13">
       <c r="A7" t="s">
         <v>17</v>
       </c>
@@ -1337,8 +1366,12 @@
       <c r="K7" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="8" spans="1:12">
+      <c r="M7">
+        <f t="shared" ca="1" si="0"/>
+        <v>1308</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13">
       <c r="A8" t="s">
         <v>18</v>
       </c>
@@ -1372,8 +1405,12 @@
       <c r="K8" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="9" spans="1:12">
+      <c r="M8">
+        <f t="shared" ca="1" si="0"/>
+        <v>1194</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13">
       <c r="A9" t="s">
         <v>19</v>
       </c>
@@ -1407,8 +1444,12 @@
       <c r="K9" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="10" spans="1:12">
+      <c r="M9">
+        <f t="shared" ca="1" si="0"/>
+        <v>1747</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13">
       <c r="A10" t="s">
         <v>19</v>
       </c>
@@ -1442,8 +1483,12 @@
       <c r="K10" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="11" spans="1:12">
+      <c r="M10">
+        <f t="shared" ca="1" si="0"/>
+        <v>1114</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13">
       <c r="A11" t="s">
         <v>19</v>
       </c>
@@ -1477,8 +1522,12 @@
       <c r="K11" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="12" spans="1:12">
+      <c r="M11">
+        <f t="shared" ca="1" si="0"/>
+        <v>1661</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13">
       <c r="A12" t="s">
         <v>19</v>
       </c>
@@ -1512,8 +1561,12 @@
       <c r="K12" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="13" spans="1:12">
+      <c r="M12">
+        <f t="shared" ca="1" si="0"/>
+        <v>1643</v>
+      </c>
+    </row>
+    <row r="13" spans="1:13">
       <c r="A13" t="s">
         <v>20</v>
       </c>
@@ -1547,8 +1600,12 @@
       <c r="K13" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="14" spans="1:12">
+      <c r="M13">
+        <f t="shared" ca="1" si="0"/>
+        <v>1057</v>
+      </c>
+    </row>
+    <row r="14" spans="1:13">
       <c r="A14" t="s">
         <v>21</v>
       </c>
@@ -1582,8 +1639,12 @@
       <c r="K14" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="15" spans="1:12">
+      <c r="M14">
+        <f t="shared" ca="1" si="0"/>
+        <v>1913</v>
+      </c>
+    </row>
+    <row r="15" spans="1:13">
       <c r="A15" t="s">
         <v>22</v>
       </c>
@@ -1617,8 +1678,12 @@
       <c r="K15" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="16" spans="1:12">
+      <c r="M15">
+        <f t="shared" ca="1" si="0"/>
+        <v>1816</v>
+      </c>
+    </row>
+    <row r="16" spans="1:13">
       <c r="A16" t="s">
         <v>22</v>
       </c>
@@ -1652,8 +1717,12 @@
       <c r="K16" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="17" spans="1:11">
+      <c r="M16">
+        <f t="shared" ca="1" si="0"/>
+        <v>1929</v>
+      </c>
+    </row>
+    <row r="17" spans="1:13">
       <c r="A17" t="s">
         <v>23</v>
       </c>
@@ -1687,8 +1756,12 @@
       <c r="K17" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="18" spans="1:11">
+      <c r="M17">
+        <f t="shared" ca="1" si="0"/>
+        <v>1982</v>
+      </c>
+    </row>
+    <row r="18" spans="1:13">
       <c r="A18" t="s">
         <v>23</v>
       </c>
@@ -1722,8 +1795,12 @@
       <c r="K18" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="19" spans="1:11">
+      <c r="M18">
+        <f t="shared" ca="1" si="0"/>
+        <v>1402</v>
+      </c>
+    </row>
+    <row r="19" spans="1:13">
       <c r="A19" t="s">
         <v>23</v>
       </c>
@@ -1757,8 +1834,12 @@
       <c r="K19" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="20" spans="1:11">
+      <c r="M19">
+        <f t="shared" ca="1" si="0"/>
+        <v>1069</v>
+      </c>
+    </row>
+    <row r="20" spans="1:13">
       <c r="A20" t="s">
         <v>23</v>
       </c>
@@ -1792,8 +1873,12 @@
       <c r="K20" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="21" spans="1:11">
+      <c r="M20">
+        <f t="shared" ca="1" si="0"/>
+        <v>1028</v>
+      </c>
+    </row>
+    <row r="21" spans="1:13">
       <c r="A21" t="s">
         <v>24</v>
       </c>
@@ -1827,8 +1912,12 @@
       <c r="K21" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="22" spans="1:11">
+      <c r="M21">
+        <f t="shared" ca="1" si="0"/>
+        <v>1054</v>
+      </c>
+    </row>
+    <row r="22" spans="1:13">
       <c r="A22" t="s">
         <v>25</v>
       </c>
@@ -1862,8 +1951,12 @@
       <c r="K22" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="23" spans="1:11">
+      <c r="M22">
+        <f t="shared" ca="1" si="0"/>
+        <v>1404</v>
+      </c>
+    </row>
+    <row r="23" spans="1:13">
       <c r="A23" t="s">
         <v>25</v>
       </c>
@@ -1897,8 +1990,12 @@
       <c r="K23" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="24" spans="1:11">
+      <c r="M23">
+        <f t="shared" ca="1" si="0"/>
+        <v>1833</v>
+      </c>
+    </row>
+    <row r="24" spans="1:13">
       <c r="A24" t="s">
         <v>26</v>
       </c>
@@ -1932,8 +2029,12 @@
       <c r="K24" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="25" spans="1:11">
+      <c r="M24">
+        <f t="shared" ca="1" si="0"/>
+        <v>1534</v>
+      </c>
+    </row>
+    <row r="25" spans="1:13">
       <c r="A25" t="s">
         <v>26</v>
       </c>
@@ -1967,8 +2068,12 @@
       <c r="K25" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="26" spans="1:11">
+      <c r="M25">
+        <f t="shared" ca="1" si="0"/>
+        <v>1985</v>
+      </c>
+    </row>
+    <row r="26" spans="1:13">
       <c r="A26" t="s">
         <v>27</v>
       </c>
@@ -2002,8 +2107,12 @@
       <c r="K26" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="27" spans="1:11">
+      <c r="M26">
+        <f t="shared" ca="1" si="0"/>
+        <v>1624</v>
+      </c>
+    </row>
+    <row r="27" spans="1:13">
       <c r="A27" t="s">
         <v>28</v>
       </c>
@@ -2037,8 +2146,12 @@
       <c r="K27" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="28" spans="1:11">
+      <c r="M27">
+        <f t="shared" ca="1" si="0"/>
+        <v>1253</v>
+      </c>
+    </row>
+    <row r="28" spans="1:13">
       <c r="A28" t="s">
         <v>29</v>
       </c>
@@ -2072,8 +2185,12 @@
       <c r="K28" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="29" spans="1:11">
+      <c r="M28">
+        <f t="shared" ca="1" si="0"/>
+        <v>1776</v>
+      </c>
+    </row>
+    <row r="29" spans="1:13">
       <c r="A29" t="s">
         <v>29</v>
       </c>
@@ -2107,8 +2224,12 @@
       <c r="K29" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="30" spans="1:11">
+      <c r="M29">
+        <f t="shared" ca="1" si="0"/>
+        <v>1405</v>
+      </c>
+    </row>
+    <row r="30" spans="1:13">
       <c r="A30" t="s">
         <v>30</v>
       </c>
@@ -2142,8 +2263,12 @@
       <c r="K30" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="31" spans="1:11">
+      <c r="M30">
+        <f t="shared" ca="1" si="0"/>
+        <v>1580</v>
+      </c>
+    </row>
+    <row r="31" spans="1:13">
       <c r="A31" t="s">
         <v>30</v>
       </c>
@@ -2177,8 +2302,12 @@
       <c r="K31" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="32" spans="1:11">
+      <c r="M31">
+        <f t="shared" ca="1" si="0"/>
+        <v>1875</v>
+      </c>
+    </row>
+    <row r="32" spans="1:13">
       <c r="A32" t="s">
         <v>31</v>
       </c>
@@ -2212,8 +2341,12 @@
       <c r="K32" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="33" spans="1:11">
+      <c r="M32">
+        <f t="shared" ca="1" si="0"/>
+        <v>1479</v>
+      </c>
+    </row>
+    <row r="33" spans="1:13">
       <c r="A33" t="s">
         <v>32</v>
       </c>
@@ -2247,8 +2380,12 @@
       <c r="K33" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="34" spans="1:11">
+      <c r="M33">
+        <f t="shared" ca="1" si="0"/>
+        <v>1735</v>
+      </c>
+    </row>
+    <row r="34" spans="1:13">
       <c r="A34" t="s">
         <v>32</v>
       </c>
@@ -2282,8 +2419,12 @@
       <c r="K34" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="35" spans="1:11">
+      <c r="M34">
+        <f t="shared" ca="1" si="0"/>
+        <v>1943</v>
+      </c>
+    </row>
+    <row r="35" spans="1:13">
       <c r="A35" t="s">
         <v>32</v>
       </c>
@@ -2317,8 +2458,12 @@
       <c r="K35" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="36" spans="1:11">
+      <c r="M35">
+        <f t="shared" ca="1" si="0"/>
+        <v>1532</v>
+      </c>
+    </row>
+    <row r="36" spans="1:13">
       <c r="A36" t="s">
         <v>33</v>
       </c>
@@ -2352,8 +2497,12 @@
       <c r="K36" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="37" spans="1:11">
+      <c r="M36">
+        <f t="shared" ca="1" si="0"/>
+        <v>1630</v>
+      </c>
+    </row>
+    <row r="37" spans="1:13">
       <c r="A37" t="s">
         <v>34</v>
       </c>
@@ -2387,8 +2536,12 @@
       <c r="K37" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="38" spans="1:11">
+      <c r="M37">
+        <f t="shared" ca="1" si="0"/>
+        <v>1320</v>
+      </c>
+    </row>
+    <row r="38" spans="1:13">
       <c r="A38" t="s">
         <v>35</v>
       </c>
@@ -2422,8 +2575,12 @@
       <c r="K38" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="39" spans="1:11">
+      <c r="M38">
+        <f t="shared" ca="1" si="0"/>
+        <v>1310</v>
+      </c>
+    </row>
+    <row r="39" spans="1:13">
       <c r="A39" t="s">
         <v>36</v>
       </c>
@@ -2457,8 +2614,12 @@
       <c r="K39" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="40" spans="1:11">
+      <c r="M39">
+        <f t="shared" ca="1" si="0"/>
+        <v>1170</v>
+      </c>
+    </row>
+    <row r="40" spans="1:13">
       <c r="A40" t="s">
         <v>36</v>
       </c>
@@ -2492,8 +2653,12 @@
       <c r="K40" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="41" spans="1:11">
+      <c r="M40">
+        <f t="shared" ca="1" si="0"/>
+        <v>1150</v>
+      </c>
+    </row>
+    <row r="41" spans="1:13">
       <c r="A41" t="s">
         <v>36</v>
       </c>
@@ -2527,8 +2692,12 @@
       <c r="K41" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="42" spans="1:11">
+      <c r="M41">
+        <f t="shared" ca="1" si="0"/>
+        <v>1119</v>
+      </c>
+    </row>
+    <row r="42" spans="1:13">
       <c r="A42" t="s">
         <v>37</v>
       </c>
@@ -2562,8 +2731,12 @@
       <c r="K42" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="43" spans="1:11">
+      <c r="M42">
+        <f t="shared" ca="1" si="0"/>
+        <v>1632</v>
+      </c>
+    </row>
+    <row r="43" spans="1:13">
       <c r="A43" t="s">
         <v>38</v>
       </c>
@@ -2597,8 +2770,12 @@
       <c r="K43" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="44" spans="1:11">
+      <c r="M43">
+        <f t="shared" ca="1" si="0"/>
+        <v>1618</v>
+      </c>
+    </row>
+    <row r="44" spans="1:13">
       <c r="A44" t="s">
         <v>38</v>
       </c>
@@ -2632,8 +2809,12 @@
       <c r="K44" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="45" spans="1:11">
+      <c r="M44">
+        <f t="shared" ca="1" si="0"/>
+        <v>1038</v>
+      </c>
+    </row>
+    <row r="45" spans="1:13">
       <c r="A45" t="s">
         <v>39</v>
       </c>
@@ -2667,8 +2848,12 @@
       <c r="K45" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="46" spans="1:11">
+      <c r="M45">
+        <f t="shared" ca="1" si="0"/>
+        <v>1876</v>
+      </c>
+    </row>
+    <row r="46" spans="1:13">
       <c r="A46" t="s">
         <v>39</v>
       </c>
@@ -2702,8 +2887,12 @@
       <c r="K46" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="47" spans="1:11">
+      <c r="M46">
+        <f t="shared" ca="1" si="0"/>
+        <v>1200</v>
+      </c>
+    </row>
+    <row r="47" spans="1:13">
       <c r="A47" t="s">
         <v>40</v>
       </c>
@@ -2737,8 +2926,12 @@
       <c r="K47" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="48" spans="1:11">
+      <c r="M47">
+        <f t="shared" ca="1" si="0"/>
+        <v>1717</v>
+      </c>
+    </row>
+    <row r="48" spans="1:13">
       <c r="A48" t="s">
         <v>41</v>
       </c>
@@ -2772,8 +2965,12 @@
       <c r="K48" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="49" spans="1:12">
+      <c r="M48">
+        <f t="shared" ca="1" si="0"/>
+        <v>1109</v>
+      </c>
+    </row>
+    <row r="49" spans="1:13">
       <c r="A49" t="s">
         <v>42</v>
       </c>
@@ -2807,8 +3004,12 @@
       <c r="K49" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="50" spans="1:12">
+      <c r="M49">
+        <f t="shared" ca="1" si="0"/>
+        <v>1635</v>
+      </c>
+    </row>
+    <row r="50" spans="1:13">
       <c r="A50" t="s">
         <v>43</v>
       </c>
@@ -2842,8 +3043,12 @@
       <c r="K50" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="51" spans="1:12">
+      <c r="M50">
+        <f t="shared" ca="1" si="0"/>
+        <v>1814</v>
+      </c>
+    </row>
+    <row r="51" spans="1:13">
       <c r="A51" t="s">
         <v>44</v>
       </c>
@@ -2878,8 +3083,12 @@
       <c r="L51" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="52" spans="1:12">
+      <c r="M51">
+        <f t="shared" ca="1" si="0"/>
+        <v>1159</v>
+      </c>
+    </row>
+    <row r="52" spans="1:13">
       <c r="B52" s="1">
         <v>44405</v>
       </c>
@@ -2913,8 +3122,12 @@
       <c r="L52" t="s">
         <v>46</v>
       </c>
-    </row>
-    <row r="53" spans="1:12">
+      <c r="M52">
+        <f t="shared" ca="1" si="0"/>
+        <v>1530</v>
+      </c>
+    </row>
+    <row r="53" spans="1:13">
       <c r="A53" t="s">
         <v>44</v>
       </c>
@@ -2948,8 +3161,12 @@
       <c r="L53" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="54" spans="1:12">
+      <c r="M53">
+        <f t="shared" ca="1" si="0"/>
+        <v>1353</v>
+      </c>
+    </row>
+    <row r="54" spans="1:13">
       <c r="A54" t="s">
         <v>44</v>
       </c>
@@ -2983,8 +3200,12 @@
       <c r="L54" t="s">
         <v>48</v>
       </c>
-    </row>
-    <row r="55" spans="1:12">
+      <c r="M54">
+        <f t="shared" ca="1" si="0"/>
+        <v>1900</v>
+      </c>
+    </row>
+    <row r="55" spans="1:13">
       <c r="A55" t="s">
         <v>44</v>
       </c>
@@ -3015,8 +3236,12 @@
       <c r="L55" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="56" spans="1:12">
+      <c r="M55">
+        <f t="shared" ca="1" si="0"/>
+        <v>1739</v>
+      </c>
+    </row>
+    <row r="56" spans="1:13">
       <c r="A56" t="s">
         <v>44</v>
       </c>
@@ -3047,8 +3272,12 @@
       <c r="L56" t="s">
         <v>50</v>
       </c>
-    </row>
-    <row r="57" spans="1:12">
+      <c r="M56">
+        <f t="shared" ca="1" si="0"/>
+        <v>1723</v>
+      </c>
+    </row>
+    <row r="57" spans="1:13">
       <c r="A57" t="s">
         <v>44</v>
       </c>
@@ -3079,8 +3308,12 @@
       <c r="L57" t="s">
         <v>51</v>
       </c>
-    </row>
-    <row r="58" spans="1:12">
+      <c r="M57">
+        <f t="shared" ca="1" si="0"/>
+        <v>1997</v>
+      </c>
+    </row>
+    <row r="58" spans="1:13">
       <c r="A58" t="s">
         <v>44</v>
       </c>
@@ -3111,8 +3344,12 @@
       <c r="L58" t="s">
         <v>52</v>
       </c>
-    </row>
-    <row r="59" spans="1:12">
+      <c r="M58">
+        <f t="shared" ca="1" si="0"/>
+        <v>1847</v>
+      </c>
+    </row>
+    <row r="59" spans="1:13">
       <c r="A59" t="s">
         <v>44</v>
       </c>
@@ -3143,8 +3380,12 @@
       <c r="L59" t="s">
         <v>53</v>
       </c>
-    </row>
-    <row r="60" spans="1:12">
+      <c r="M59">
+        <f t="shared" ca="1" si="0"/>
+        <v>1312</v>
+      </c>
+    </row>
+    <row r="60" spans="1:13">
       <c r="A60" t="s">
         <v>44</v>
       </c>
@@ -3175,8 +3416,12 @@
       <c r="L60" t="s">
         <v>54</v>
       </c>
-    </row>
-    <row r="61" spans="1:12">
+      <c r="M60">
+        <f t="shared" ca="1" si="0"/>
+        <v>1168</v>
+      </c>
+    </row>
+    <row r="61" spans="1:13">
       <c r="A61" t="s">
         <v>44</v>
       </c>
@@ -3207,8 +3452,12 @@
       <c r="L61" t="s">
         <v>55</v>
       </c>
-    </row>
-    <row r="62" spans="1:12">
+      <c r="M61">
+        <f t="shared" ca="1" si="0"/>
+        <v>1850</v>
+      </c>
+    </row>
+    <row r="62" spans="1:13">
       <c r="A62" t="s">
         <v>44</v>
       </c>
@@ -3239,8 +3488,12 @@
       <c r="L62" t="s">
         <v>56</v>
       </c>
-    </row>
-    <row r="63" spans="1:12">
+      <c r="M62">
+        <f t="shared" ca="1" si="0"/>
+        <v>1314</v>
+      </c>
+    </row>
+    <row r="63" spans="1:13">
       <c r="A63" t="s">
         <v>44</v>
       </c>
@@ -3274,8 +3527,13 @@
       <c r="L63" t="s">
         <v>57</v>
       </c>
+      <c r="M63">
+        <f t="shared" ca="1" si="0"/>
+        <v>1985</v>
+      </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -3289,15 +3547,15 @@
       <selection pane="bottomLeft" activeCell="O11" sqref="O11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="16.5"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="15.125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.25" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.25" customWidth="1"/>
-    <col min="6" max="6" width="10.875" style="2" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="15.1640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.1640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.1640625" customWidth="1"/>
+    <col min="6" max="6" width="10.83203125" style="2" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="11" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="13.125" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="19.25" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="13.1640625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="19.1640625" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="11" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -5126,6 +5384,7 @@
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="O2:O1048568">
     <sortCondition ref="O2:O1048568"/>
   </sortState>
+  <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -5138,12 +5397,12 @@
       <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
   <cols>
     <col min="5" max="5" width="9.5" style="1" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" ht="16.5">
+    <row r="1" spans="1:17">
       <c r="A1" t="s">
         <v>102</v>
       </c>
@@ -5196,7 +5455,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="2" spans="1:17" ht="16.5">
+    <row r="2" spans="1:17">
       <c r="B2" t="s">
         <v>118</v>
       </c>
@@ -5216,7 +5475,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:17" ht="16.5">
+    <row r="3" spans="1:17">
       <c r="A3">
         <v>4</v>
       </c>
@@ -5239,7 +5498,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:17" ht="16.5">
+    <row r="4" spans="1:17">
       <c r="A4">
         <v>5</v>
       </c>
@@ -5262,7 +5521,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:17" ht="16.5">
+    <row r="5" spans="1:17">
       <c r="A5">
         <v>10</v>
       </c>
@@ -5285,7 +5544,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:17" ht="16.5">
+    <row r="6" spans="1:17">
       <c r="A6">
         <v>15</v>
       </c>
@@ -5308,7 +5567,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:17" ht="16.5">
+    <row r="7" spans="1:17">
       <c r="A7">
         <v>16</v>
       </c>
@@ -5331,7 +5590,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:17" ht="16.5">
+    <row r="8" spans="1:17">
       <c r="A8">
         <v>17</v>
       </c>
@@ -5354,7 +5613,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:17" ht="16.5">
+    <row r="9" spans="1:17">
       <c r="A9">
         <v>18</v>
       </c>
@@ -5377,7 +5636,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:17" ht="16.5">
+    <row r="10" spans="1:17">
       <c r="A10">
         <v>19</v>
       </c>
@@ -5400,7 +5659,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:17" ht="16.5">
+    <row r="11" spans="1:17">
       <c r="A11">
         <v>20</v>
       </c>
@@ -5423,7 +5682,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:17" ht="16.5">
+    <row r="12" spans="1:17">
       <c r="A12">
         <v>21</v>
       </c>
@@ -5446,7 +5705,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:17" ht="16.5">
+    <row r="13" spans="1:17">
       <c r="A13">
         <v>25</v>
       </c>
@@ -5469,7 +5728,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:17" ht="16.5">
+    <row r="14" spans="1:17">
       <c r="A14">
         <v>26</v>
       </c>
@@ -5492,7 +5751,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:17" ht="16.5">
+    <row r="15" spans="1:17">
       <c r="A15">
         <v>28</v>
       </c>
@@ -5515,7 +5774,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:17" ht="16.5">
+    <row r="16" spans="1:17">
       <c r="A16">
         <v>29</v>
       </c>
@@ -5538,7 +5797,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="1:13" ht="16.5">
+    <row r="17" spans="1:13">
       <c r="A17">
         <v>30</v>
       </c>
@@ -5561,7 +5820,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="1:13" ht="16.5">
+    <row r="18" spans="1:13">
       <c r="A18">
         <v>31</v>
       </c>
@@ -5584,7 +5843,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="19" spans="1:13" ht="16.5">
+    <row r="19" spans="1:13">
       <c r="A19">
         <v>32</v>
       </c>
@@ -5607,7 +5866,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="20" spans="1:13" ht="16.5">
+    <row r="20" spans="1:13">
       <c r="A20">
         <v>33</v>
       </c>
@@ -5630,7 +5889,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="21" spans="1:13" ht="16.5">
+    <row r="21" spans="1:13">
       <c r="A21">
         <v>34</v>
       </c>
@@ -5653,7 +5912,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="22" spans="1:13" ht="16.5">
+    <row r="22" spans="1:13">
       <c r="A22">
         <v>36</v>
       </c>
@@ -5676,7 +5935,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="23" spans="1:13" ht="16.5">
+    <row r="23" spans="1:13">
       <c r="A23">
         <v>40</v>
       </c>
@@ -5699,7 +5958,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="24" spans="1:13" ht="16.5">
+    <row r="24" spans="1:13">
       <c r="A24">
         <v>41</v>
       </c>
@@ -5722,7 +5981,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="25" spans="1:13" ht="16.5">
+    <row r="25" spans="1:13">
       <c r="A25">
         <v>42</v>
       </c>
@@ -5745,7 +6004,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="26" spans="1:13" ht="16.5">
+    <row r="26" spans="1:13">
       <c r="A26">
         <v>43</v>
       </c>
@@ -5768,7 +6027,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="27" spans="1:13" ht="16.5">
+    <row r="27" spans="1:13">
       <c r="A27">
         <v>47</v>
       </c>
@@ -5791,7 +6050,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="28" spans="1:13" ht="16.5">
+    <row r="28" spans="1:13">
       <c r="A28">
         <v>50</v>
       </c>
@@ -5814,7 +6073,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="29" spans="1:13" ht="16.5">
+    <row r="29" spans="1:13">
       <c r="A29">
         <v>51</v>
       </c>
@@ -5837,7 +6096,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="30" spans="1:13" ht="16.5">
+    <row r="30" spans="1:13">
       <c r="A30">
         <v>57</v>
       </c>
@@ -5860,7 +6119,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="31" spans="1:13" ht="16.5">
+    <row r="31" spans="1:13">
       <c r="A31">
         <v>59</v>
       </c>
@@ -5883,7 +6142,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="32" spans="1:13" ht="16.5">
+    <row r="32" spans="1:13">
       <c r="A32">
         <v>60</v>
       </c>
@@ -5906,7 +6165,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="33" spans="1:13" ht="16.5">
+    <row r="33" spans="1:13">
       <c r="A33">
         <v>63</v>
       </c>
@@ -5929,7 +6188,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="34" spans="1:13" ht="16.5">
+    <row r="34" spans="1:13">
       <c r="A34">
         <v>64</v>
       </c>
@@ -5952,7 +6211,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="35" spans="1:13" ht="16.5">
+    <row r="35" spans="1:13">
       <c r="A35">
         <v>71</v>
       </c>
@@ -5975,7 +6234,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="36" spans="1:13" ht="16.5">
+    <row r="36" spans="1:13">
       <c r="A36">
         <v>72</v>
       </c>
@@ -5998,7 +6257,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="37" spans="1:13" ht="16.5">
+    <row r="37" spans="1:13">
       <c r="A37">
         <v>73</v>
       </c>
@@ -6021,7 +6280,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="38" spans="1:13" ht="16.5">
+    <row r="38" spans="1:13">
       <c r="A38">
         <v>78</v>
       </c>
@@ -6044,7 +6303,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="39" spans="1:13" ht="16.5">
+    <row r="39" spans="1:13">
       <c r="A39">
         <v>79</v>
       </c>
@@ -6067,7 +6326,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="40" spans="1:13" ht="16.5">
+    <row r="40" spans="1:13">
       <c r="A40">
         <v>80</v>
       </c>
@@ -6090,7 +6349,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="41" spans="1:13" ht="16.5">
+    <row r="41" spans="1:13">
       <c r="A41">
         <v>82</v>
       </c>
@@ -6113,7 +6372,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="42" spans="1:13" ht="16.5">
+    <row r="42" spans="1:13">
       <c r="A42">
         <v>83</v>
       </c>
@@ -6136,7 +6395,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="43" spans="1:13" ht="16.5">
+    <row r="43" spans="1:13">
       <c r="A43">
         <v>84</v>
       </c>
@@ -6159,7 +6418,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="44" spans="1:13" ht="16.5">
+    <row r="44" spans="1:13">
       <c r="A44">
         <v>85</v>
       </c>
@@ -6182,7 +6441,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="45" spans="1:13" ht="16.5">
+    <row r="45" spans="1:13">
       <c r="A45">
         <v>86</v>
       </c>
@@ -6205,7 +6464,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="46" spans="1:13" ht="16.5">
+    <row r="46" spans="1:13">
       <c r="A46">
         <v>90</v>
       </c>
@@ -6228,7 +6487,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="47" spans="1:13" ht="16.5">
+    <row r="47" spans="1:13">
       <c r="A47">
         <v>95</v>
       </c>
@@ -6251,7 +6510,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="48" spans="1:13" ht="16.5">
+    <row r="48" spans="1:13">
       <c r="A48">
         <v>97</v>
       </c>
@@ -6274,7 +6533,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="49" spans="1:13" ht="16.5">
+    <row r="49" spans="1:13">
       <c r="A49">
         <v>98</v>
       </c>
@@ -6297,7 +6556,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="50" spans="1:13" ht="16.5">
+    <row r="50" spans="1:13">
       <c r="A50">
         <v>99</v>
       </c>
@@ -6320,7 +6579,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="51" spans="1:13" ht="16.5">
+    <row r="51" spans="1:13">
       <c r="A51">
         <v>1</v>
       </c>
@@ -6343,7 +6602,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="52" spans="1:13" ht="16.5">
+    <row r="52" spans="1:13">
       <c r="A52">
         <v>2</v>
       </c>
@@ -6366,7 +6625,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="53" spans="1:13" ht="16.5">
+    <row r="53" spans="1:13">
       <c r="A53">
         <v>6</v>
       </c>
@@ -6389,7 +6648,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="54" spans="1:13" ht="16.5">
+    <row r="54" spans="1:13">
       <c r="A54">
         <v>7</v>
       </c>
@@ -6412,7 +6671,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="55" spans="1:13" ht="16.5">
+    <row r="55" spans="1:13">
       <c r="A55">
         <v>8</v>
       </c>
@@ -6435,7 +6694,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="56" spans="1:13" ht="16.5">
+    <row r="56" spans="1:13">
       <c r="A56">
         <v>9</v>
       </c>
@@ -6458,7 +6717,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="57" spans="1:13" ht="16.5">
+    <row r="57" spans="1:13">
       <c r="A57">
         <v>11</v>
       </c>
@@ -6481,7 +6740,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="58" spans="1:13" ht="16.5">
+    <row r="58" spans="1:13">
       <c r="A58">
         <v>12</v>
       </c>
@@ -6504,7 +6763,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="59" spans="1:13" ht="16.5">
+    <row r="59" spans="1:13">
       <c r="A59">
         <v>13</v>
       </c>
@@ -6527,7 +6786,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="60" spans="1:13" ht="16.5">
+    <row r="60" spans="1:13">
       <c r="A60">
         <v>14</v>
       </c>
@@ -6550,7 +6809,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="61" spans="1:13" ht="16.5">
+    <row r="61" spans="1:13">
       <c r="A61">
         <v>22</v>
       </c>
@@ -6573,7 +6832,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="62" spans="1:13" ht="16.5">
+    <row r="62" spans="1:13">
       <c r="A62">
         <v>23</v>
       </c>
@@ -6596,7 +6855,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="63" spans="1:13" ht="16.5">
+    <row r="63" spans="1:13">
       <c r="A63">
         <v>24</v>
       </c>
@@ -6619,7 +6878,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="64" spans="1:13" ht="16.5">
+    <row r="64" spans="1:13">
       <c r="A64">
         <v>27</v>
       </c>
@@ -6642,7 +6901,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="65" spans="1:13" ht="16.5">
+    <row r="65" spans="1:13">
       <c r="A65">
         <v>35</v>
       </c>
@@ -6665,7 +6924,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="66" spans="1:13" ht="16.5">
+    <row r="66" spans="1:13">
       <c r="A66">
         <v>37</v>
       </c>
@@ -6688,7 +6947,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="67" spans="1:13" ht="16.5">
+    <row r="67" spans="1:13">
       <c r="A67">
         <v>38</v>
       </c>
@@ -6711,7 +6970,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="68" spans="1:13" ht="16.5">
+    <row r="68" spans="1:13">
       <c r="A68">
         <v>39</v>
       </c>
@@ -6734,7 +6993,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="69" spans="1:13" ht="16.5">
+    <row r="69" spans="1:13">
       <c r="A69">
         <v>44</v>
       </c>
@@ -6757,7 +7016,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="70" spans="1:13" ht="16.5">
+    <row r="70" spans="1:13">
       <c r="A70">
         <v>45</v>
       </c>
@@ -6780,7 +7039,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="71" spans="1:13" ht="16.5">
+    <row r="71" spans="1:13">
       <c r="A71">
         <v>46</v>
       </c>
@@ -6803,7 +7062,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="72" spans="1:13" ht="16.5">
+    <row r="72" spans="1:13">
       <c r="A72">
         <v>48</v>
       </c>
@@ -6826,7 +7085,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="73" spans="1:13" ht="16.5">
+    <row r="73" spans="1:13">
       <c r="A73">
         <v>49</v>
       </c>
@@ -6849,7 +7108,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="74" spans="1:13" ht="16.5">
+    <row r="74" spans="1:13">
       <c r="A74">
         <v>52</v>
       </c>
@@ -6872,7 +7131,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="75" spans="1:13" ht="16.5">
+    <row r="75" spans="1:13">
       <c r="A75">
         <v>53</v>
       </c>
@@ -6895,7 +7154,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="76" spans="1:13" ht="16.5">
+    <row r="76" spans="1:13">
       <c r="A76">
         <v>54</v>
       </c>
@@ -6918,7 +7177,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="77" spans="1:13" ht="16.5">
+    <row r="77" spans="1:13">
       <c r="A77">
         <v>55</v>
       </c>
@@ -6941,7 +7200,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="78" spans="1:13" ht="16.5">
+    <row r="78" spans="1:13">
       <c r="A78">
         <v>56</v>
       </c>
@@ -6964,7 +7223,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="79" spans="1:13" ht="16.5">
+    <row r="79" spans="1:13">
       <c r="A79">
         <v>58</v>
       </c>
@@ -6987,7 +7246,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="80" spans="1:13" ht="16.5">
+    <row r="80" spans="1:13">
       <c r="A80">
         <v>61</v>
       </c>
@@ -7010,7 +7269,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="81" spans="1:13" ht="16.5">
+    <row r="81" spans="1:13">
       <c r="A81">
         <v>62</v>
       </c>
@@ -7033,7 +7292,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="82" spans="1:13" ht="16.5">
+    <row r="82" spans="1:13">
       <c r="A82">
         <v>65</v>
       </c>
@@ -7056,7 +7315,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="83" spans="1:13" ht="16.5">
+    <row r="83" spans="1:13">
       <c r="A83">
         <v>66</v>
       </c>
@@ -7079,7 +7338,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="84" spans="1:13" ht="16.5">
+    <row r="84" spans="1:13">
       <c r="A84">
         <v>67</v>
       </c>
@@ -7102,7 +7361,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="85" spans="1:13" ht="16.5">
+    <row r="85" spans="1:13">
       <c r="A85">
         <v>68</v>
       </c>
@@ -7125,7 +7384,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="86" spans="1:13" ht="16.5">
+    <row r="86" spans="1:13">
       <c r="A86">
         <v>69</v>
       </c>
@@ -7148,7 +7407,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="87" spans="1:13" ht="16.5">
+    <row r="87" spans="1:13">
       <c r="A87">
         <v>70</v>
       </c>
@@ -7171,7 +7430,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="88" spans="1:13" ht="16.5">
+    <row r="88" spans="1:13">
       <c r="A88">
         <v>74</v>
       </c>
@@ -7194,7 +7453,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="89" spans="1:13" ht="16.5">
+    <row r="89" spans="1:13">
       <c r="A89">
         <v>75</v>
       </c>
@@ -7217,7 +7476,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="90" spans="1:13" ht="16.5">
+    <row r="90" spans="1:13">
       <c r="A90">
         <v>76</v>
       </c>
@@ -7240,7 +7499,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="91" spans="1:13" ht="16.5">
+    <row r="91" spans="1:13">
       <c r="A91">
         <v>77</v>
       </c>
@@ -7263,7 +7522,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="92" spans="1:13" ht="16.5">
+    <row r="92" spans="1:13">
       <c r="A92">
         <v>81</v>
       </c>
@@ -7286,7 +7545,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="93" spans="1:13" ht="16.5">
+    <row r="93" spans="1:13">
       <c r="A93">
         <v>87</v>
       </c>
@@ -7309,7 +7568,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="94" spans="1:13" ht="16.5">
+    <row r="94" spans="1:13">
       <c r="A94">
         <v>88</v>
       </c>
@@ -7332,7 +7591,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="95" spans="1:13" ht="16.5">
+    <row r="95" spans="1:13">
       <c r="A95">
         <v>89</v>
       </c>
@@ -7355,7 +7614,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="96" spans="1:13" ht="16.5">
+    <row r="96" spans="1:13">
       <c r="A96">
         <v>91</v>
       </c>
@@ -7378,7 +7637,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="97" spans="1:13" ht="16.5">
+    <row r="97" spans="1:13">
       <c r="A97">
         <v>92</v>
       </c>
@@ -7401,7 +7660,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="98" spans="1:13" ht="16.5">
+    <row r="98" spans="1:13">
       <c r="A98">
         <v>93</v>
       </c>
@@ -7424,7 +7683,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="99" spans="1:13" ht="16.5">
+    <row r="99" spans="1:13">
       <c r="A99">
         <v>94</v>
       </c>
@@ -7447,7 +7706,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="100" spans="1:13" ht="16.5">
+    <row r="100" spans="1:13">
       <c r="A100">
         <v>96</v>
       </c>
@@ -7470,7 +7729,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="101" spans="1:13" ht="16.5">
+    <row r="101" spans="1:13">
       <c r="A101">
         <v>100</v>
       </c>
@@ -7497,6 +7756,7 @@
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:Q101">
     <sortCondition ref="M2:M101"/>
   </sortState>
+  <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>